<commit_message>
Accreditamento Winsap cs Anatomia Patologica #7
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap_CS
subject_application_version: 20.17.00
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.17.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.17.00/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/CS_SESSIONE_20250418/Winsap_CS/20.17.00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit-my.sharepoint.com/personal/francesco_navarra_eng_it/Documents/Desktop/CDA2/CS_SESSIONE_20250512/Winsap_CS/20.17.00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71CB2A62-BE90-45BA-8D69-BFB08AE7F5EB}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A26A1A38-3400-48C4-A2A7-EA2A39C5FE17}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="474">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1360,15 +1360,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-03-19T12:28:31Z</t>
-  </si>
-  <si>
-    <t>62800d3fd629a362</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.65348d142b9ed6590b99096d8fc73df132dcec320c81e438d3517397d330acbc.69ef7191df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.1 v2.80, Codes: PROVA]</t>
   </si>
   <si>
@@ -1399,15 +1390,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-03-19T12:37:19Z</t>
-  </si>
-  <si>
-    <t>dfd31bb8ed8e2c69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.8aa65fe0bf3c5e0ce900afd644a792555726ac91a2e2155122acb3ff03a1673b.fc1bbeb4d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b28| Sezione Epicrisi: La sezione DEVE contenere l'elemento text obbligatorio.]</t>
   </si>
   <si>
@@ -1418,15 +1400,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-03-19T12:45:11Z</t>
-  </si>
-  <si>
-    <t>be9de617cefd9f6d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.eddbefe96295f3a6f2df77bd0b5b07bf5983c7ceec6d11496400b47899efb45e.4fd7e45a89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b195| Sezione Diagnosi: L'elemento entry/organizer/component/observation (Linfonodi) deve avere l'elemento value con @xsi:type='IVL_PQ', che identifica il numero dei linfonodi.]</t>
   </si>
   <si>
@@ -1437,15 +1410,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-03-19T12:49:46Z</t>
-  </si>
-  <si>
-    <t>d86d6f8b7bb9d73f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.708e6ca4f0b0b6c4293abf91a756334d99cc657b79a9bce461dc82f031aa4a60.eaf9bd5822^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b69| Sotto-sezione Anamnesi (entry Anamnesi familiare): L'elemento entry/organizer/subject/relatedSubject deve contenere l'elemento code.]</t>
   </si>
   <si>
@@ -1456,15 +1420,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-03-19T13:15:11Z</t>
-  </si>
-  <si>
-    <t>798e2dcf628f2502</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.fff62558a274e6d3ba3f54fe7788e0a4e6fc806b99fb17f569a2b089d601b1f4.510d53dd30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b103| SSotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime è obbligatorio.]</t>
   </si>
   <si>
@@ -1473,15 +1428,6 @@
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2025-03-19T14:14:34Z</t>
-  </si>
-  <si>
-    <t>f165cd04a98368a4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.8564f4e9a85138f133549caf1f740d24ee30e697ebb3abcd68c0f2af718ab2ca.711fd05147^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: PROVA]</t>
@@ -1790,40 +1736,91 @@
     <t>subject_application_vendor:Engineering Ingegneria Informatica SpA</t>
   </si>
   <si>
-    <t>2025-04-18T11:06:20Z</t>
-  </si>
-  <si>
-    <t>8b5da3f5062fa2731c83da80b384cd94</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1000000.a213157dfbf4c9c78bb959bf0a4d9e18161f5a7eade5b8458b050c4df3c0b977.cb5c86867d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-04-18T10:17:38Z</t>
-  </si>
-  <si>
-    <t>af3a3ff04d7b3cbdcfd3bd0358dfb53e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.33f11191dc0436e58d3978581bc8818b18e46665257f64a1cb5f7e04dbddfac0.e25c014b57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-04-18T10:21:04Z</t>
-  </si>
-  <si>
-    <t>35126f97641ba4744dc1b64bdfb5f02b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.fc688e55d0747f453a02a7e936d255e300fa2d3a07c548b8b212e597c01b0d99.5e61601573^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-04-18T10:32:34Z</t>
-  </si>
-  <si>
-    <t>1328ffa01a5feb1621b7ab1c3e66bce4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1000000.cade55a9ed607a81c1f30b944d00db6385773fe008ad8b1ca34005a6ace240da.6ea630541b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-12T14:48:22Z</t>
+  </si>
+  <si>
+    <t>44e3ebab565408d15828085c8926b7b4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.dddaaf6cfc6cfbd9062b54e962b7ef05a4c9e3a60ee7fd9ec38d95e27ec798d9.e432f7fbf8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T14:59:50Z</t>
+  </si>
+  <si>
+    <t>669eb6851664d07a81c58c30eb76963b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.867ccf0ae50fe6a5d10f39a1ecc7aaa55d1ddea0af05348fa9acc93486f360ad.57282926f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T15:08:37Z</t>
+  </si>
+  <si>
+    <t>d763fcafc199667e5356b39349996ccb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1000000.1227a0eb8e9841e4b93211b9f2acdbff5d6fe30e0eb73106ecad54854439d320.a67f3ebc65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T15:28:03Z</t>
+  </si>
+  <si>
+    <t>e144e238214398f4d973c2770a467897</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1000000.2246f8d31740df3c521966f31807da294e2ee47691b8cef912fcb781859427ce.a934d9613b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T15:46:03Z</t>
+  </si>
+  <si>
+    <t>332ad2eff902cabdc8e1696548aff58d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.ffcc1a1d984c6995009ce8883e76ea9905f87988de50bb44f5f8e24163e8cf52.805f9f5dab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3f7d3983801cffc1758e8233bc2e9e55</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.8198544c6a0dbda270b604d7b45b42c7ff66be03ebd200359e3afebc2b38de4d.5f89756cc9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T16:10:44Z</t>
+  </si>
+  <si>
+    <t>79c91c0eee9e7b30560723a6d1bd1ff5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.88a24e27dd44e32a91a0f09f03deddf8226216c9576de564e9c8f52f856a5ff1.0b4a0ad17a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T16:19:27Z</t>
+  </si>
+  <si>
+    <t>c23cd5c4e9b9b4befce6f397dd480436</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.2c034757403e570ee0bea670909421bb316d2591772d61c96c408bbc9e55f7e3.ac91d51d9c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T16:31:42Z</t>
+  </si>
+  <si>
+    <t>696b9cf4ef95d03eaead4d8da174a934</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.8e53f0c36f103d32aa6373f5da7e742af452a58a1f6b99e3ac01ca8a3e6aefa1.875c20fc28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-12T16:43:07Z</t>
+  </si>
+  <si>
+    <t>03299a6afedb736c0afa667c563b517f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.6fd5311f19dd953d091b5543964e1ed6737f8422a7eee0c00c6c70cc689da9d2.61cc39a942^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3888,10 +3885,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F149" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I181" sqref="I181"/>
+      <selection pane="bottomRight" activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3964,7 +3961,7 @@
       </c>
       <c r="B3" s="51"/>
       <c r="C3" s="56" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="D3" s="48"/>
       <c r="F3" s="6"/>
@@ -3990,7 +3987,7 @@
       <c r="A4" s="52"/>
       <c r="B4" s="53"/>
       <c r="C4" s="56" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="4"/>
@@ -4017,7 +4014,7 @@
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="56" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="D5" s="48"/>
       <c r="F5" s="6"/>
@@ -9389,16 +9386,16 @@
         <v>316</v>
       </c>
       <c r="F150" s="33">
-        <v>45765</v>
+        <v>45789</v>
       </c>
       <c r="G150" s="33" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="H150" s="33" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="I150" s="39" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="J150" s="29" t="s">
         <v>76</v>
@@ -9436,16 +9433,16 @@
         <v>318</v>
       </c>
       <c r="F151" s="33">
-        <v>45765</v>
+        <v>45789</v>
       </c>
       <c r="G151" s="33" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="H151" s="33" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="I151" s="39" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="J151" s="29" t="s">
         <v>76</v>
@@ -9483,16 +9480,16 @@
         <v>320</v>
       </c>
       <c r="F152" s="33">
-        <v>45765</v>
+        <v>45789</v>
       </c>
       <c r="G152" s="33" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="H152" s="33" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="I152" s="39" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="J152" s="29" t="s">
         <v>76</v>
@@ -9714,16 +9711,16 @@
         <v>331</v>
       </c>
       <c r="F157" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G157" s="33" t="s">
-        <v>332</v>
+        <v>457</v>
       </c>
       <c r="H157" s="33" t="s">
-        <v>333</v>
+        <v>458</v>
       </c>
       <c r="I157" s="39" t="s">
-        <v>334</v>
+        <v>459</v>
       </c>
       <c r="J157" s="29" t="s">
         <v>76</v>
@@ -9737,7 +9734,7 @@
         <v>76</v>
       </c>
       <c r="O157" s="29" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="P157" s="29" t="s">
         <v>76</v>
@@ -9749,7 +9746,7 @@
         <v>322</v>
       </c>
       <c r="S157" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T157" s="29"/>
       <c r="U157" s="34"/>
@@ -9769,10 +9766,10 @@
         <v>314</v>
       </c>
       <c r="D158" s="31" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F158" s="33"/>
       <c r="G158" s="33"/>
@@ -9810,10 +9807,10 @@
         <v>314</v>
       </c>
       <c r="D159" s="31" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E159" s="32" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F159" s="33"/>
       <c r="G159" s="33"/>
@@ -9823,7 +9820,7 @@
         <v>322</v>
       </c>
       <c r="K159" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L159" s="29"/>
       <c r="M159" s="29"/>
@@ -9851,22 +9848,22 @@
         <v>314</v>
       </c>
       <c r="D160" s="31" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E160" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F160" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G160" s="33" t="s">
-        <v>344</v>
+        <v>457</v>
       </c>
       <c r="H160" s="33" t="s">
-        <v>345</v>
+        <v>460</v>
       </c>
       <c r="I160" s="39" t="s">
-        <v>346</v>
+        <v>461</v>
       </c>
       <c r="J160" s="29" t="s">
         <v>76</v>
@@ -9880,7 +9877,7 @@
         <v>76</v>
       </c>
       <c r="O160" s="29" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="P160" s="29" t="s">
         <v>76</v>
@@ -9892,7 +9889,7 @@
         <v>322</v>
       </c>
       <c r="S160" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T160" s="29"/>
       <c r="U160" s="34"/>
@@ -9912,22 +9909,22 @@
         <v>314</v>
       </c>
       <c r="D161" s="31" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E161" s="32" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F161" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G161" s="33" t="s">
-        <v>350</v>
+        <v>462</v>
       </c>
       <c r="H161" s="33" t="s">
-        <v>351</v>
+        <v>463</v>
       </c>
       <c r="I161" s="39" t="s">
-        <v>352</v>
+        <v>464</v>
       </c>
       <c r="J161" s="29" t="s">
         <v>76</v>
@@ -9941,7 +9938,7 @@
         <v>76</v>
       </c>
       <c r="O161" s="29" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="P161" s="29" t="s">
         <v>76</v>
@@ -9953,7 +9950,7 @@
         <v>322</v>
       </c>
       <c r="S161" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T161" s="29"/>
       <c r="U161" s="34"/>
@@ -9973,22 +9970,22 @@
         <v>314</v>
       </c>
       <c r="D162" s="31" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="E162" s="32" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F162" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>356</v>
+        <v>465</v>
       </c>
       <c r="H162" s="33" t="s">
-        <v>357</v>
+        <v>466</v>
       </c>
       <c r="I162" s="39" t="s">
-        <v>358</v>
+        <v>467</v>
       </c>
       <c r="J162" s="29" t="s">
         <v>76</v>
@@ -10002,7 +9999,7 @@
         <v>76</v>
       </c>
       <c r="O162" s="29" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="P162" s="29" t="s">
         <v>76</v>
@@ -10014,7 +10011,7 @@
         <v>322</v>
       </c>
       <c r="S162" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T162" s="29"/>
       <c r="U162" s="34"/>
@@ -10034,22 +10031,22 @@
         <v>314</v>
       </c>
       <c r="D163" s="31" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="E163" s="32" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="F163" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G163" s="33" t="s">
-        <v>362</v>
+        <v>468</v>
       </c>
       <c r="H163" s="33" t="s">
-        <v>363</v>
+        <v>469</v>
       </c>
       <c r="I163" s="39" t="s">
-        <v>364</v>
+        <v>470</v>
       </c>
       <c r="J163" s="29" t="s">
         <v>76</v>
@@ -10063,7 +10060,7 @@
         <v>76</v>
       </c>
       <c r="O163" s="29" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="P163" s="29" t="s">
         <v>76</v>
@@ -10075,7 +10072,7 @@
         <v>322</v>
       </c>
       <c r="S163" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T163" s="29"/>
       <c r="U163" s="34"/>
@@ -10095,22 +10092,22 @@
         <v>314</v>
       </c>
       <c r="D164" s="31" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="E164" s="32" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="F164" s="33">
-        <v>45735</v>
+        <v>45789</v>
       </c>
       <c r="G164" s="33" t="s">
-        <v>368</v>
+        <v>471</v>
       </c>
       <c r="H164" s="33" t="s">
-        <v>369</v>
+        <v>472</v>
       </c>
       <c r="I164" s="39" t="s">
-        <v>370</v>
+        <v>473</v>
       </c>
       <c r="J164" s="29" t="s">
         <v>76</v>
@@ -10124,7 +10121,7 @@
         <v>76</v>
       </c>
       <c r="O164" s="29" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="P164" s="29" t="s">
         <v>76</v>
@@ -10136,7 +10133,7 @@
         <v>322</v>
       </c>
       <c r="S164" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T164" s="29"/>
       <c r="U164" s="34"/>
@@ -10156,10 +10153,10 @@
         <v>314</v>
       </c>
       <c r="D165" s="31" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="E165" s="32" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="F165" s="33"/>
       <c r="G165" s="33"/>
@@ -10169,7 +10166,7 @@
         <v>322</v>
       </c>
       <c r="K165" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L165" s="29"/>
       <c r="M165" s="29"/>
@@ -10197,10 +10194,10 @@
         <v>53</v>
       </c>
       <c r="D166" s="31" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="E166" s="32" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="F166" s="33"/>
       <c r="G166" s="33"/>
@@ -10234,10 +10231,10 @@
         <v>53</v>
       </c>
       <c r="D167" s="31" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="E167" s="32" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="F167" s="33"/>
       <c r="G167" s="33"/>
@@ -10271,10 +10268,10 @@
         <v>55</v>
       </c>
       <c r="D168" s="31" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="E168" s="32" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="F168" s="33"/>
       <c r="G168" s="33"/>
@@ -10308,10 +10305,10 @@
         <v>55</v>
       </c>
       <c r="D169" s="31" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="E169" s="32" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="F169" s="33"/>
       <c r="G169" s="33"/>
@@ -10345,10 +10342,10 @@
         <v>57</v>
       </c>
       <c r="D170" s="31" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="E170" s="32" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="F170" s="33"/>
       <c r="G170" s="33"/>
@@ -10382,10 +10379,10 @@
         <v>57</v>
       </c>
       <c r="D171" s="31" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="E171" s="32" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="F171" s="33"/>
       <c r="G171" s="33"/>
@@ -10419,10 +10416,10 @@
         <v>51</v>
       </c>
       <c r="D172" s="31" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="E172" s="32" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="F172" s="33"/>
       <c r="G172" s="33"/>
@@ -10456,10 +10453,10 @@
         <v>51</v>
       </c>
       <c r="D173" s="31" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="E173" s="32" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="F173" s="33"/>
       <c r="G173" s="33"/>
@@ -10493,10 +10490,10 @@
         <v>44</v>
       </c>
       <c r="D174" s="31" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="E174" s="32" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="F174" s="33"/>
       <c r="G174" s="33"/>
@@ -10530,10 +10527,10 @@
         <v>63</v>
       </c>
       <c r="D175" s="31" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="E175" s="32" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="F175" s="33"/>
       <c r="G175" s="33"/>
@@ -10567,10 +10564,10 @@
         <v>63</v>
       </c>
       <c r="D176" s="31" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="E176" s="32" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="F176" s="33"/>
       <c r="G176" s="33"/>
@@ -10604,10 +10601,10 @@
         <v>61</v>
       </c>
       <c r="D177" s="31" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="E177" s="32" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="F177" s="33"/>
       <c r="G177" s="33"/>
@@ -10641,10 +10638,10 @@
         <v>61</v>
       </c>
       <c r="D178" s="31" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="E178" s="32" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="F178" s="33"/>
       <c r="G178" s="33"/>
@@ -10678,10 +10675,10 @@
         <v>59</v>
       </c>
       <c r="D179" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="E179" s="32" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="F179" s="33"/>
       <c r="G179" s="33"/>
@@ -10715,10 +10712,10 @@
         <v>59</v>
       </c>
       <c r="D180" s="31" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="E180" s="32" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="F180" s="33"/>
       <c r="G180" s="33"/>
@@ -10752,22 +10749,22 @@
         <v>314</v>
       </c>
       <c r="D181" s="31" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="E181" s="32" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="F181" s="33">
-        <v>45765</v>
+        <v>45789</v>
       </c>
       <c r="G181" s="33" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="H181" s="33" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="I181" s="39" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="J181" s="29" t="s">
         <v>76</v>
@@ -10799,10 +10796,10 @@
         <v>57</v>
       </c>
       <c r="D182" s="31" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="E182" s="31" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="F182" s="31"/>
       <c r="G182" s="31"/>
@@ -10836,10 +10833,10 @@
         <v>55</v>
       </c>
       <c r="D183" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="E183" s="29" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="F183" s="31"/>
       <c r="G183" s="31"/>
@@ -10873,10 +10870,10 @@
         <v>63</v>
       </c>
       <c r="D184" s="31" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="E184" s="29" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="F184" s="31"/>
       <c r="G184" s="31"/>
@@ -10910,10 +10907,10 @@
         <v>59</v>
       </c>
       <c r="D185" s="31" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="E185" s="32" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="F185" s="31"/>
       <c r="G185" s="31"/>
@@ -10947,10 +10944,10 @@
         <v>61</v>
       </c>
       <c r="D186" s="31" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="E186" s="32" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="F186" s="31"/>
       <c r="G186" s="31"/>
@@ -10984,10 +10981,10 @@
         <v>44</v>
       </c>
       <c r="D187" s="31" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="E187" s="32" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="F187" s="31"/>
       <c r="G187" s="31"/>
@@ -11021,10 +11018,10 @@
         <v>51</v>
       </c>
       <c r="D188" s="31" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="E188" s="29" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="F188" s="31"/>
       <c r="G188" s="31"/>
@@ -11058,10 +11055,10 @@
         <v>57</v>
       </c>
       <c r="D189" s="31" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="E189" s="29" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="F189" s="31"/>
       <c r="G189" s="31"/>
@@ -11095,10 +11092,10 @@
         <v>53</v>
       </c>
       <c r="D190" s="31" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="E190" s="29" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="F190" s="31"/>
       <c r="G190" s="31"/>
@@ -11132,10 +11129,10 @@
         <v>314</v>
       </c>
       <c r="D191" s="31" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="E191" s="29" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="F191" s="31"/>
       <c r="G191" s="31"/>
@@ -11145,7 +11142,7 @@
         <v>322</v>
       </c>
       <c r="K191" s="31" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="L191" s="31"/>
       <c r="M191" s="31"/>
@@ -15338,17 +15335,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
@@ -15358,22 +15355,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -15403,22 +15400,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="30" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15426,13 +15423,13 @@
         <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15440,13 +15437,13 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15454,13 +15451,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C4" s="12">
         <v>446.447</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15468,13 +15465,13 @@
         <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15482,13 +15479,13 @@
         <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.6" x14ac:dyDescent="0.4">
@@ -15496,13 +15493,13 @@
         <v>63</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.6" x14ac:dyDescent="0.4">
@@ -15510,13 +15507,13 @@
         <v>57</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.6" x14ac:dyDescent="0.4">
@@ -15524,27 +15521,27 @@
         <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" s="41" t="s">
         <v>437</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -15552,13 +15549,13 @@
         <v>314</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -16544,7 +16541,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>76</v>
@@ -16552,7 +16549,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>322</v>
@@ -17569,12 +17566,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17773,20 +17772,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17811,12 +17811,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Accreditamento Winsap cs Anatomia Patologica #9
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap_CS
subject_application_version: 20.17.00
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.17.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.17.00/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit-my.sharepoint.com/personal/francesco_navarra_eng_it/Documents/Desktop/CDA2/CS_SESSIONE_20250512/Winsap_CS/20.17.00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/CS_SESSIONE_20250514/Winsap_CS/20.17.00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A26A1A38-3400-48C4-A2A7-EA2A39C5FE17}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF475BEE-320F-41DC-8BCF-755042C0828F}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1736,42 +1736,6 @@
     <t>subject_application_vendor:Engineering Ingegneria Informatica SpA</t>
   </si>
   <si>
-    <t>2025-05-12T14:48:22Z</t>
-  </si>
-  <si>
-    <t>44e3ebab565408d15828085c8926b7b4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.dddaaf6cfc6cfbd9062b54e962b7ef05a4c9e3a60ee7fd9ec38d95e27ec798d9.e432f7fbf8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-05-12T14:59:50Z</t>
-  </si>
-  <si>
-    <t>669eb6851664d07a81c58c30eb76963b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1.867ccf0ae50fe6a5d10f39a1ecc7aaa55d1ddea0af05348fa9acc93486f360ad.57282926f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-05-12T15:08:37Z</t>
-  </si>
-  <si>
-    <t>d763fcafc199667e5356b39349996ccb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1000000.1227a0eb8e9841e4b93211b9f2acdbff5d6fe30e0eb73106ecad54854439d320.a67f3ebc65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-05-12T15:28:03Z</t>
-  </si>
-  <si>
-    <t>e144e238214398f4d973c2770a467897</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.1000000.2246f8d31740df3c521966f31807da294e2ee47691b8cef912fcb781859427ce.a934d9613b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-05-12T15:46:03Z</t>
   </si>
   <si>
@@ -1821,6 +1785,42 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.1.6fd5311f19dd953d091b5543964e1ed6737f8422a7eee0c00c6c70cc689da9d2.61cc39a942^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-14T15:54:09Z</t>
+  </si>
+  <si>
+    <t>3aa681d913da64b6bdd6256682715a23</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.43b18ca001d7a961ef0740dad71af15969debddfbea33bcc8f37487b22acb9ed.d0920b1ca2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-14T15:57:33Z</t>
+  </si>
+  <si>
+    <t>0f550c4ebfd0321e772557521e8fd347</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1.0b8a7a0bf44dadafbecc51bf8966e1487114cde65181d2f242e1bfdbfc58021a.7bb1e582f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-14T16:01:31Z</t>
+  </si>
+  <si>
+    <t>5c7c652decb9655f20bb2186418c4236</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1000000.633985c8f021459252c8a3b25e760df85f046aec4832201a053e45fe61c615c4.872013fd2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-14T16:03:10Z</t>
+  </si>
+  <si>
+    <t>b74d389b8cfe2d9b077665c9280d71b6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.1000000.a2c8d50074a7ab5c8bd433079af44f04db4b24a947b7bb8eb7f0cac017d15d51.ecfa9c439b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3888,7 +3888,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="E149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I164" sqref="I164"/>
+      <selection pane="bottomRight" activeCell="I181" sqref="I181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -9386,16 +9386,16 @@
         <v>316</v>
       </c>
       <c r="F150" s="33">
-        <v>45789</v>
+        <v>45791</v>
       </c>
       <c r="G150" s="33" t="s">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="H150" s="33" t="s">
-        <v>446</v>
+        <v>463</v>
       </c>
       <c r="I150" s="39" t="s">
-        <v>447</v>
+        <v>464</v>
       </c>
       <c r="J150" s="29" t="s">
         <v>76</v>
@@ -9433,16 +9433,16 @@
         <v>318</v>
       </c>
       <c r="F151" s="33">
-        <v>45789</v>
+        <v>45791</v>
       </c>
       <c r="G151" s="33" t="s">
-        <v>448</v>
+        <v>465</v>
       </c>
       <c r="H151" s="33" t="s">
-        <v>449</v>
+        <v>466</v>
       </c>
       <c r="I151" s="39" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="J151" s="29" t="s">
         <v>76</v>
@@ -9480,16 +9480,16 @@
         <v>320</v>
       </c>
       <c r="F152" s="33">
-        <v>45789</v>
+        <v>45791</v>
       </c>
       <c r="G152" s="33" t="s">
-        <v>451</v>
+        <v>468</v>
       </c>
       <c r="H152" s="33" t="s">
-        <v>452</v>
+        <v>469</v>
       </c>
       <c r="I152" s="39" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="J152" s="29" t="s">
         <v>76</v>
@@ -9714,13 +9714,13 @@
         <v>45789</v>
       </c>
       <c r="G157" s="33" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="H157" s="33" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="I157" s="39" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="J157" s="29" t="s">
         <v>76</v>
@@ -9857,13 +9857,13 @@
         <v>45789</v>
       </c>
       <c r="G160" s="33" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="H160" s="33" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="I160" s="39" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="J160" s="29" t="s">
         <v>76</v>
@@ -9918,13 +9918,13 @@
         <v>45789</v>
       </c>
       <c r="G161" s="33" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H161" s="33" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="I161" s="39" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="J161" s="29" t="s">
         <v>76</v>
@@ -9979,13 +9979,13 @@
         <v>45789</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="H162" s="33" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="I162" s="39" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="J162" s="29" t="s">
         <v>76</v>
@@ -10040,13 +10040,13 @@
         <v>45789</v>
       </c>
       <c r="G163" s="33" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="H163" s="33" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="I163" s="39" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="J163" s="29" t="s">
         <v>76</v>
@@ -10101,13 +10101,13 @@
         <v>45789</v>
       </c>
       <c r="G164" s="33" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="H164" s="33" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="I164" s="39" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="J164" s="29" t="s">
         <v>76</v>
@@ -10755,16 +10755,16 @@
         <v>387</v>
       </c>
       <c r="F181" s="33">
-        <v>45789</v>
+        <v>45791</v>
       </c>
       <c r="G181" s="33" t="s">
-        <v>454</v>
+        <v>471</v>
       </c>
       <c r="H181" s="33" t="s">
-        <v>455</v>
+        <v>472</v>
       </c>
       <c r="I181" s="39" t="s">
-        <v>456</v>
+        <v>473</v>
       </c>
       <c r="J181" s="29" t="s">
         <v>76</v>
@@ -17566,14 +17566,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17772,21 +17770,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17811,9 +17808,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>